<commit_message>
Modified data. Added multiple degree plans for members
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533708\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533708\Desktop\WebApplication2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="87">
   <si>
     <t>DegreeID</t>
   </si>
@@ -158,15 +158,6 @@
     <t>DCID</t>
   </si>
   <si>
-    <t>DPID</t>
-  </si>
-  <si>
-    <t>DPAbbr</t>
-  </si>
-  <si>
-    <t>DPName</t>
-  </si>
-  <si>
     <t>StudentID</t>
   </si>
   <si>
@@ -290,7 +281,16 @@
     <t>Summer 2021</t>
   </si>
   <si>
-    <t>DPS</t>
+    <t>DegreePlanID</t>
+  </si>
+  <si>
+    <t>DegreePlanAbbr</t>
+  </si>
+  <si>
+    <t>DegreePlanName</t>
+  </si>
+  <si>
+    <t>DegreePlanSelected</t>
   </si>
 </sst>
 </file>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,7 +1018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -1574,35 +1574,35 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="17.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="5" max="5" width="18.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1614,12 +1614,12 @@
         <v>533568</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="3">
+        <v>67</v>
+      </c>
+      <c r="E2" s="2">
         <v>5681</v>
       </c>
     </row>
@@ -1628,16 +1628,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>533708</v>
+        <v>533568</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" s="3">
-        <v>7082</v>
+        <v>68</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5682</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1645,20 +1645,75 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
+        <v>533708</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="2">
+        <v>7081</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>533708</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="2">
+        <v>7082</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
         <v>533897</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="C6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="2">
+        <v>8971</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>533897</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="2">
         <v>8973</v>
       </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1681,13 +1736,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="D1" s="3">
         <v>919</v>
@@ -1698,10 +1753,10 @@
         <v>533568</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D2" s="3">
         <v>919569870</v>
@@ -1712,10 +1767,10 @@
         <v>533708</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D3" s="3">
         <v>919571315</v>
@@ -1726,10 +1781,10 @@
         <v>533897</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D4" s="3">
         <v>919571233</v>
@@ -1744,31 +1799,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="130" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView zoomScale="130" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="2" width="19.140625" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>86</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1785,7 +1841,7 @@
         <v>542</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1802,7 +1858,7 @@
         <v>563</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1819,7 +1875,7 @@
         <v>560</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1836,7 +1892,7 @@
         <v>664</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1853,7 +1909,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1870,7 +1926,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1887,7 +1943,7 @@
         <v>618</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1904,7 +1960,7 @@
         <v>691</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1921,7 +1977,7 @@
         <v>692</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1938,7 +1994,7 @@
         <v>20</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1955,7 +2011,7 @@
         <v>555</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1972,7 +2028,7 @@
         <v>542</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1989,7 +2045,7 @@
         <v>563</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2006,7 +2062,7 @@
         <v>560</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2023,7 +2079,7 @@
         <v>664</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2040,7 +2096,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2057,7 +2113,7 @@
         <v>10</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2074,7 +2130,7 @@
         <v>618</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2091,7 +2147,7 @@
         <v>691</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2108,7 +2164,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2125,7 +2181,7 @@
         <v>692</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2142,7 +2198,7 @@
         <v>555</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2159,7 +2215,7 @@
         <v>542</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2176,7 +2232,7 @@
         <v>563</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2193,7 +2249,7 @@
         <v>560</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2210,7 +2266,7 @@
         <v>664</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2227,7 +2283,7 @@
         <v>6</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2244,7 +2300,7 @@
         <v>10</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2261,7 +2317,7 @@
         <v>20</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2278,7 +2334,7 @@
         <v>555</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2295,7 +2351,7 @@
         <v>691</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2312,7 +2368,7 @@
         <v>618</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2329,7 +2385,7 @@
         <v>692</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2341,7 +2397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2355,19 +2411,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2381,10 +2437,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2398,10 +2454,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2415,10 +2471,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2432,10 +2488,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2449,10 +2505,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2466,10 +2522,10 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2483,10 +2539,10 @@
         <v>3</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2500,10 +2556,10 @@
         <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2517,10 +2573,10 @@
         <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2534,10 +2590,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2551,10 +2607,10 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2568,10 +2624,10 @@
         <v>3</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2585,10 +2641,10 @@
         <v>4</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed 919 to _919N
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533708\Desktop\WebApplication2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533897\Documents\SEMESTER 2\C#.NET\MVCapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="88">
   <si>
     <t>DegreeID</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>DegreePlanSelected</t>
+  </si>
+  <si>
+    <t>_919N</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -1721,8 +1724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1744,8 +1747,8 @@
       <c r="C1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="3">
-        <v>919</v>
+      <c r="D1" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changed DC to DegreeCreditID in xls
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533897\Documents\SEMESTER 2\C#.NET\MVCapp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533708\Desktop\DotNetProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -155,9 +155,6 @@
     <t>Elective 2</t>
   </si>
   <si>
-    <t>DCID</t>
-  </si>
-  <si>
     <t>StudentID</t>
   </si>
   <si>
@@ -294,6 +291,9 @@
   </si>
   <si>
     <t>_919N</t>
+  </si>
+  <si>
+    <t>DegreeCreditID</t>
   </si>
 </sst>
 </file>
@@ -1021,19 +1021,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="19.28515625" style="2" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1594,19 +1594,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1617,10 +1617,10 @@
         <v>533568</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E2" s="2">
         <v>5681</v>
@@ -1634,10 +1634,10 @@
         <v>533568</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E3" s="2">
         <v>5682</v>
@@ -1651,10 +1651,10 @@
         <v>533708</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E4" s="2">
         <v>7081</v>
@@ -1668,10 +1668,10 @@
         <v>533708</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2">
         <v>7082</v>
@@ -1685,10 +1685,10 @@
         <v>533897</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" s="2">
         <v>8971</v>
@@ -1702,10 +1702,10 @@
         <v>533897</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="E7" s="2">
         <v>8973</v>
@@ -1724,7 +1724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1739,16 +1739,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1756,10 +1756,10 @@
         <v>533568</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="D2" s="3">
         <v>919569870</v>
@@ -1770,10 +1770,10 @@
         <v>533708</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="D3" s="3">
         <v>919571315</v>
@@ -1784,10 +1784,10 @@
         <v>533897</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="D4" s="3">
         <v>919571233</v>
@@ -1815,19 +1815,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1844,7 +1844,7 @@
         <v>542</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1861,7 +1861,7 @@
         <v>563</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1878,7 +1878,7 @@
         <v>560</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1895,7 +1895,7 @@
         <v>664</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1912,7 +1912,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1929,7 +1929,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1946,7 +1946,7 @@
         <v>618</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1963,7 +1963,7 @@
         <v>691</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1980,7 +1980,7 @@
         <v>692</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1997,7 +1997,7 @@
         <v>20</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2014,7 +2014,7 @@
         <v>555</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2031,7 +2031,7 @@
         <v>542</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2048,7 +2048,7 @@
         <v>563</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2065,7 +2065,7 @@
         <v>560</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2082,7 +2082,7 @@
         <v>664</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2099,7 +2099,7 @@
         <v>6</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2116,7 +2116,7 @@
         <v>10</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2133,7 +2133,7 @@
         <v>618</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2150,7 +2150,7 @@
         <v>691</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2167,7 +2167,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2184,7 +2184,7 @@
         <v>692</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2201,7 +2201,7 @@
         <v>555</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2218,7 +2218,7 @@
         <v>542</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2235,7 +2235,7 @@
         <v>563</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2252,7 +2252,7 @@
         <v>560</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2269,7 +2269,7 @@
         <v>664</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2286,7 +2286,7 @@
         <v>6</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2303,7 +2303,7 @@
         <v>10</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2320,7 +2320,7 @@
         <v>20</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2337,7 +2337,7 @@
         <v>555</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2354,7 +2354,7 @@
         <v>691</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2371,7 +2371,7 @@
         <v>618</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2388,7 +2388,7 @@
         <v>692</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2414,19 +2414,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2440,10 +2440,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2457,10 +2457,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2474,10 +2474,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2491,10 +2491,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2508,10 +2508,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2525,10 +2525,10 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2542,10 +2542,10 @@
         <v>3</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2559,10 +2559,10 @@
         <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2576,10 +2576,10 @@
         <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2593,10 +2593,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2610,10 +2610,10 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2627,10 +2627,10 @@
         <v>3</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2644,10 +2644,10 @@
         <v>4</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committed with Excel data new column addition for formula Created DbInitializer.cs Added seeding for Degrees, StudentTerms
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
   <si>
     <t>DegreeID</t>
   </si>
@@ -41,9 +41,6 @@
     <t>MS ACS+2</t>
   </si>
   <si>
-    <t>DegreeAbbr(U,8)</t>
-  </si>
-  <si>
     <t>ACS+DB</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>MS ACS</t>
   </si>
   <si>
-    <t>DegreeName(U,20)</t>
-  </si>
-  <si>
     <t>NumberOfTerms</t>
   </si>
   <si>
@@ -290,10 +284,19 @@
     <t>DegreePlanSelected</t>
   </si>
   <si>
-    <t>_919N</t>
-  </si>
-  <si>
     <t>DegreeCreditID</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>DegreeAbbr</t>
+  </si>
+  <si>
+    <t>DegreeName</t>
+  </si>
+  <si>
+    <t>N919</t>
   </si>
 </sst>
 </file>
@@ -626,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,21 +643,24 @@
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>3</v>
+        <v>86</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -667,47 +673,63 @@
       <c r="D2" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="str">
+        <f>"new Degree {" &amp;$A$1 &amp;" = " &amp;A2 &amp; ", " &amp;$B$1 &amp; "='" &amp;B2  &amp; "', " &amp;$C$1 &amp; "='" &amp;C2 &amp;"'}"</f>
+        <v>new Degree {DegreeID = 1, DegreeAbbr='ACS+2', DegreeName='MS ACS+2'}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E5" si="0">"new Degree {" &amp;$A$1 &amp;" = " &amp;A3 &amp; ", " &amp;$B$1 &amp; "='" &amp;B3  &amp; "', " &amp;$C$1 &amp; "='" &amp;C3 &amp;"'"</f>
+        <v>new Degree {DegreeID = 2, DegreeAbbr='ACS+DB', DegreeName='MS ACS+DB'</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>new Degree {DegreeID = 3, DegreeAbbr='ACS+NF', DegreeName='MS ACS+NF'</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>new Degree {DegreeID = 4, DegreeAbbr='ACS', DegreeName='MS ACS'</v>
       </c>
     </row>
   </sheetData>
@@ -718,10 +740,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,38 +751,43 @@
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="12.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="4" max="6" width="9.140625" style="3"/>
+    <col min="7" max="7" width="107.85546875" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>460</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -771,16 +798,20 @@
       <c r="F2" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="str">
+        <f>"new Credit {" &amp;$A$1 &amp;"=" &amp;A2 &amp; ", " &amp;$B$1 &amp;"='" &amp;B2 &amp; "', " &amp;$C$1 &amp;"='" &amp;C2 &amp; "', "&amp;$D$1 &amp;"=" &amp;D2 &amp; ", "&amp;$E$1 &amp;"=" &amp;E2 &amp; ", " &amp;$F$1 &amp;"=" &amp;F2 &amp;"}"</f>
+        <v>new Credit {CreditID=460, CreditAbbr='DB', CreditName='Databases', IsSummer=0, IsSpring=1, IsFall=1}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>356</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
@@ -791,8 +822,12 @@
       <c r="F3" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="3" t="str">
+        <f t="shared" ref="G3:G14" si="0">"new Credit {" &amp;$A$1 &amp;"=" &amp;A3 &amp; ", " &amp;$B$1 &amp;"='" &amp;B3 &amp; "', " &amp;$C$1 &amp;"='" &amp;C3 &amp; "', "&amp;$D$1 &amp;"=" &amp;D3 &amp; ", "&amp;$E$1 &amp;"=" &amp;E3 &amp; ", " &amp;$F$1 &amp;"=" &amp;F3 &amp;"}"</f>
+        <v>new Credit {CreditID=356, CreditAbbr='NF', CreditName='Network Fundamentals', IsSummer=0, IsSpring=1, IsFall=1}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>542</v>
       </c>
@@ -800,7 +835,7 @@
         <v>542</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -811,8 +846,12 @@
       <c r="F4" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Credit {CreditID=542, CreditAbbr='542', CreditName='OOPS with Java', IsSummer=0, IsSpring=1, IsFall=1}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>563</v>
       </c>
@@ -820,7 +859,7 @@
         <v>563</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -831,8 +870,12 @@
       <c r="F5" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Credit {CreditID=563, CreditAbbr='563', CreditName='Web Apps', IsSummer=0, IsSpring=1, IsFall=1}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>560</v>
       </c>
@@ -840,7 +883,7 @@
         <v>560</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
@@ -851,16 +894,20 @@
       <c r="F6" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Credit {CreditID=560, CreditAbbr='560', CreditName='Advanced Databases', IsSummer=1, IsSpring=1, IsFall=1}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>664</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -871,16 +918,20 @@
       <c r="F7" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Credit {CreditID=664, CreditAbbr='664-UX', CreditName='User Experience', IsSummer=0, IsSpring=1, IsFall=1}</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>618</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
@@ -891,16 +942,20 @@
       <c r="F8" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Credit {CreditID=618, CreditAbbr='618-PM', CreditName='Project Management', IsSummer=1, IsSpring=0, IsFall=0}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>555</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -911,16 +966,20 @@
       <c r="F9" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Credit {CreditID=555, CreditAbbr='555-NS', CreditName='Network Security', IsSummer=0, IsSpring=1, IsFall=1}</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>691</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -931,16 +990,20 @@
       <c r="F10" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Credit {CreditID=691, CreditAbbr='691-GDP1', CreditName='GDP1', IsSummer=0, IsSpring=1, IsFall=1}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>692</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
@@ -951,16 +1014,20 @@
       <c r="F11" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Credit {CreditID=692, CreditAbbr='692-GDP2', CreditName='GDP2', IsSummer=0, IsSpring=1, IsFall=1}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12" s="3">
         <v>0</v>
@@ -971,16 +1038,20 @@
       <c r="F12" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Credit {CreditID=6, CreditAbbr='Mobile', CreditName='643 or 644 Mobile', IsSummer=0, IsSpring=1, IsFall=1}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="D13" s="3">
         <v>0</v>
@@ -991,16 +1062,20 @@
       <c r="F13" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Credit {CreditID=10, CreditAbbr='E1', CreditName='Elective 1', IsSummer=0, IsSpring=1, IsFall=1}</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>20</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="D14" s="3">
         <v>0</v>
@@ -1010,6 +1085,10 @@
       </c>
       <c r="F14" s="3">
         <v>1</v>
+      </c>
+      <c r="G14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Credit {CreditID=20, CreditAbbr='E2', CreditName='Elective 2', IsSummer=0, IsSpring=1, IsFall=1}</v>
       </c>
     </row>
   </sheetData>
@@ -1019,30 +1098,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="64.140625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1052,8 +1136,12 @@
       <c r="C2" s="3">
         <v>460</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="str">
+        <f>"new DegreeCredit {" &amp;$A$1 &amp;"=" &amp;A2 &amp; ", " &amp;$B$1 &amp;"=" &amp;B2 &amp; ", " &amp;$C$1 &amp;"=" &amp;C2 &amp;"}"</f>
+        <v>new DegreeCredit {DegreeCreditID=1, DegreeID=1, CreditID=460}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1063,8 +1151,12 @@
       <c r="C3" s="3">
         <v>356</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="str">
+        <f t="shared" ref="D3:D49" si="0">"new DegreeCredit {" &amp;$A$1 &amp;"=" &amp;A3 &amp; ", " &amp;$B$1 &amp;"=" &amp;B3 &amp; ", " &amp;$C$1 &amp;"=" &amp;C3 &amp;"}"</f>
+        <v>new DegreeCredit {DegreeCreditID=2, DegreeID=1, CreditID=356}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1074,8 +1166,12 @@
       <c r="C4" s="3">
         <v>542</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=3, DegreeID=1, CreditID=542}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1085,8 +1181,12 @@
       <c r="C5" s="3">
         <v>563</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=4, DegreeID=1, CreditID=563}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1096,8 +1196,12 @@
       <c r="C6" s="3">
         <v>560</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=5, DegreeID=1, CreditID=560}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1107,8 +1211,12 @@
       <c r="C7" s="3">
         <v>664</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=6, DegreeID=1, CreditID=664}</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1118,8 +1226,12 @@
       <c r="C8" s="3">
         <v>618</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=7, DegreeID=1, CreditID=618}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1129,8 +1241,12 @@
       <c r="C9" s="3">
         <v>555</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=8, DegreeID=1, CreditID=555}</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1140,8 +1256,12 @@
       <c r="C10" s="3">
         <v>691</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=9, DegreeID=1, CreditID=691}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1151,8 +1271,12 @@
       <c r="C11" s="3">
         <v>692</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=10, DegreeID=1, CreditID=692}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1162,8 +1286,12 @@
       <c r="C12" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=11, DegreeID=1, CreditID=6}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1173,8 +1301,12 @@
       <c r="C13" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=12, DegreeID=1, CreditID=10}</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1184,8 +1316,12 @@
       <c r="C14" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=13, DegreeID=1, CreditID=20}</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1195,8 +1331,12 @@
       <c r="C15" s="3">
         <v>460</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=14, DegreeID=2, CreditID=460}</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1206,8 +1346,12 @@
       <c r="C16" s="3">
         <v>542</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=15, DegreeID=2, CreditID=542}</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1217,8 +1361,12 @@
       <c r="C17" s="3">
         <v>563</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=16, DegreeID=2, CreditID=563}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1228,8 +1376,12 @@
       <c r="C18" s="3">
         <v>560</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=17, DegreeID=2, CreditID=560}</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1239,8 +1391,12 @@
       <c r="C19" s="3">
         <v>664</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=18, DegreeID=2, CreditID=664}</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1250,8 +1406,12 @@
       <c r="C20" s="3">
         <v>618</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=19, DegreeID=2, CreditID=618}</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1261,8 +1421,12 @@
       <c r="C21" s="3">
         <v>555</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=20, DegreeID=2, CreditID=555}</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1272,8 +1436,12 @@
       <c r="C22" s="3">
         <v>691</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=21, DegreeID=2, CreditID=691}</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1283,8 +1451,12 @@
       <c r="C23" s="3">
         <v>692</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=22, DegreeID=2, CreditID=692}</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1294,8 +1466,12 @@
       <c r="C24" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=23, DegreeID=2, CreditID=6}</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1305,8 +1481,12 @@
       <c r="C25" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=24, DegreeID=2, CreditID=10}</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1316,8 +1496,12 @@
       <c r="C26" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=25, DegreeID=2, CreditID=20}</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1327,8 +1511,12 @@
       <c r="C27" s="3">
         <v>356</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=26, DegreeID=3, CreditID=356}</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1338,8 +1526,12 @@
       <c r="C28" s="3">
         <v>542</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=27, DegreeID=3, CreditID=542}</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1349,8 +1541,12 @@
       <c r="C29" s="3">
         <v>563</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=28, DegreeID=3, CreditID=563}</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1360,8 +1556,12 @@
       <c r="C30" s="3">
         <v>560</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=29, DegreeID=3, CreditID=560}</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1371,8 +1571,12 @@
       <c r="C31" s="3">
         <v>664</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=30, DegreeID=3, CreditID=664}</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1382,8 +1586,12 @@
       <c r="C32" s="3">
         <v>618</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=31, DegreeID=3, CreditID=618}</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1393,8 +1601,12 @@
       <c r="C33" s="3">
         <v>555</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=32, DegreeID=3, CreditID=555}</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1404,8 +1616,12 @@
       <c r="C34" s="3">
         <v>691</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=33, DegreeID=3, CreditID=691}</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1415,8 +1631,12 @@
       <c r="C35" s="3">
         <v>692</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=34, DegreeID=3, CreditID=692}</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1426,8 +1646,12 @@
       <c r="C36" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=35, DegreeID=3, CreditID=6}</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1437,8 +1661,12 @@
       <c r="C37" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=36, DegreeID=3, CreditID=10}</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1448,8 +1676,12 @@
       <c r="C38" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=37, DegreeID=3, CreditID=20}</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1459,8 +1691,12 @@
       <c r="C39" s="3">
         <v>542</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=38, DegreeID=4, CreditID=542}</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1470,8 +1706,12 @@
       <c r="C40" s="3">
         <v>563</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=39, DegreeID=4, CreditID=563}</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1481,8 +1721,12 @@
       <c r="C41" s="3">
         <v>560</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=40, DegreeID=4, CreditID=560}</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1492,8 +1736,12 @@
       <c r="C42" s="3">
         <v>664</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=41, DegreeID=4, CreditID=664}</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1503,8 +1751,12 @@
       <c r="C43" s="3">
         <v>618</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=42, DegreeID=4, CreditID=618}</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1514,8 +1766,12 @@
       <c r="C44" s="3">
         <v>555</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=43, DegreeID=4, CreditID=555}</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1525,8 +1781,12 @@
       <c r="C45" s="3">
         <v>691</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=44, DegreeID=4, CreditID=691}</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1536,8 +1796,12 @@
       <c r="C46" s="3">
         <v>692</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=45, DegreeID=4, CreditID=692}</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1547,8 +1811,12 @@
       <c r="C47" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=46, DegreeID=4, CreditID=6}</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1558,8 +1826,12 @@
       <c r="C48" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=47, DegreeID=4, CreditID=10}</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1568,6 +1840,10 @@
       </c>
       <c r="C49" s="3">
         <v>20</v>
+      </c>
+      <c r="D49" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreeCredit {DegreeCreditID=48, DegreeID=4, CreditID=20}</v>
       </c>
     </row>
   </sheetData>
@@ -1577,10 +1853,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1590,26 +1866,30 @@
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1617,16 +1897,20 @@
         <v>533568</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E2" s="2">
         <v>5681</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="str">
+        <f>"new DegreePlan {" &amp;$A$1 &amp;"=" &amp;A2 &amp; ", " &amp;$B$1 &amp;"=" &amp;B2 &amp; ", " &amp;$C$1 &amp;"='" &amp;C2 &amp; "', "&amp;$D$1 &amp;"='" &amp;D2 &amp; "', "&amp;$E$1 &amp;"=" &amp;E2 &amp; "}"</f>
+        <v>new DegreePlan {DegreePlanID=1, StudentID=533568, DegreePlanAbbr='Super Fast', DegreePlanName='Cheetah', DegreePlanSelected=5681}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1634,16 +1918,20 @@
         <v>533568</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="E3" s="2">
         <v>5682</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F7" si="0">"new DegreePlan {" &amp;$A$1 &amp;"=" &amp;A3 &amp; ", " &amp;$B$1 &amp;"=" &amp;B3 &amp; ", " &amp;$C$1 &amp;"='" &amp;C3 &amp; "', "&amp;$D$1 &amp;"='" &amp;D3 &amp; "', "&amp;$E$1 &amp;"=" &amp;E3 &amp; "}"</f>
+        <v>new DegreePlan {DegreePlanID=2, StudentID=533568, DegreePlanAbbr='Slow and Easy', DegreePlanName='Tortoise', DegreePlanSelected=5682}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1651,16 +1939,20 @@
         <v>533708</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E4" s="2">
         <v>7081</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan {DegreePlanID=3, StudentID=533708, DegreePlanAbbr='Super Fast', DegreePlanName='Cheetah', DegreePlanSelected=7081}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1668,16 +1960,20 @@
         <v>533708</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="E5" s="2">
         <v>7082</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan {DegreePlanID=4, StudentID=533708, DegreePlanAbbr='Slow and Easy', DegreePlanName='Tortoise', DegreePlanSelected=7082}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1685,16 +1981,20 @@
         <v>533897</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E6" s="2">
         <v>8971</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan {DegreePlanID=5, StudentID=533897, DegreePlanAbbr='Super Fast', DegreePlanName='Cheetah', DegreePlanSelected=8971}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1702,16 +2002,20 @@
         <v>533897</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E7" s="2">
         <v>8973</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlan {DegreePlanID=6, StudentID=533897, DegreePlanAbbr='Summer Off', DegreePlanName='Rabbit', DegreePlanSelected=8973}</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="3"/>
     </row>
   </sheetData>
@@ -1722,10 +2026,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,63 +2038,79 @@
     <col min="2" max="2" width="13.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
+    <col min="5" max="5" width="88.85546875" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>533568</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D2" s="3">
         <v>919569870</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="3" t="str">
+        <f>"new Student {" &amp;$A$1 &amp;"=" &amp;A2 &amp; ", " &amp;$B$1 &amp;"='" &amp;B2 &amp; "', "&amp;$C$1 &amp;"='" &amp;C2 &amp; "', "&amp;$D$1 &amp;"=" &amp;D2 &amp;"}"</f>
+        <v>new Student {StudentID=533568, Family='Bodepudi', Given='Mallikarjuna', N919=919569870}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>533708</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" s="3">
         <v>919571315</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="str">
+        <f t="shared" ref="E3:E4" si="0">"new Student {" &amp;$A$1 &amp;"=" &amp;A3 &amp; ", " &amp;$B$1 &amp;"='" &amp;B3 &amp; "', "&amp;$C$1 &amp;"='" &amp;C3 &amp; "', "&amp;$D$1 &amp;"=" &amp;D3 &amp;"}"</f>
+        <v>new Student {StudentID=533708, Family='Kancharla', Given='Sai Krishna Teja', N919=919571315}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>533897</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D4" s="3">
         <v>919571233</v>
+      </c>
+      <c r="E4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Student {StudentID=533897, Family='Atluri', Given='Mouni Krishna', N919=919571233}</v>
       </c>
     </row>
   </sheetData>
@@ -1800,37 +2120,42 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="19.140625" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="3"/>
+    <col min="3" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="78.140625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1844,10 +2169,14 @@
         <v>542</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F2" s="3" t="str">
+        <f>"new Slot {" &amp;$A$1 &amp;"=" &amp;A2 &amp; ", " &amp;$B$1 &amp;"=" &amp;B2 &amp; ", "&amp;$C$1 &amp;"=" &amp;C2 &amp; ", "&amp;$D$1 &amp;"=" &amp;D2 &amp; ", "&amp;$E$1 &amp;"='" &amp;E2 &amp;"'}"</f>
+        <v>new Slot {SlotID=1, DegreePlanSelected=5681, Term=1, CreditID=542, Status='C'}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1861,10 +2190,14 @@
         <v>563</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F3" s="3" t="str">
+        <f t="shared" ref="F3:F34" si="0">"new Slot {" &amp;$A$1 &amp;"=" &amp;A3 &amp; ", " &amp;$B$1 &amp;"=" &amp;B3 &amp; ", "&amp;$C$1 &amp;"=" &amp;C3 &amp; ", "&amp;$D$1 &amp;"=" &amp;D3 &amp; ", "&amp;$E$1 &amp;"='" &amp;E3 &amp;"'}"</f>
+        <v>new Slot {SlotID=2, DegreePlanSelected=5681, Term=1, CreditID=563, Status='C'}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1878,10 +2211,14 @@
         <v>560</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=3, DegreePlanSelected=5681, Term=1, CreditID=560, Status='C'}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1895,10 +2232,14 @@
         <v>664</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=4, DegreePlanSelected=5681, Term=2, CreditID=664, Status='A'}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1912,10 +2253,14 @@
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=5, DegreePlanSelected=5681, Term=2, CreditID=6, Status='A'}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1929,10 +2274,14 @@
         <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=6, DegreePlanSelected=5681, Term=2, CreditID=10, Status='A'}</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1946,10 +2295,14 @@
         <v>618</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=7, DegreePlanSelected=5681, Term=3, CreditID=618, Status='P'}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1963,10 +2316,14 @@
         <v>691</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=8, DegreePlanSelected=5681, Term=3, CreditID=691, Status='P'}</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1980,10 +2337,14 @@
         <v>692</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=9, DegreePlanSelected=5681, Term=4, CreditID=692, Status='P'}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1997,10 +2358,14 @@
         <v>20</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=10, DegreePlanSelected=5681, Term=4, CreditID=20, Status='P'}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2014,10 +2379,14 @@
         <v>555</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=11, DegreePlanSelected=5681, Term=4, CreditID=555, Status='P'}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2031,10 +2400,14 @@
         <v>542</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=12, DegreePlanSelected=7082, Term=1, CreditID=542, Status='C'}</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2048,10 +2421,14 @@
         <v>563</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=13, DegreePlanSelected=7082, Term=1, CreditID=563, Status='C'}</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2065,10 +2442,14 @@
         <v>560</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=14, DegreePlanSelected=7082, Term=1, CreditID=560, Status='C'}</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2082,10 +2463,14 @@
         <v>664</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=15, DegreePlanSelected=7082, Term=2, CreditID=664, Status='A'}</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2099,10 +2484,14 @@
         <v>6</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=16, DegreePlanSelected=7082, Term=2, CreditID=6, Status='A'}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2116,10 +2505,14 @@
         <v>10</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=17, DegreePlanSelected=7082, Term=2, CreditID=10, Status='A'}</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2133,10 +2526,14 @@
         <v>618</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=18, DegreePlanSelected=7082, Term=3, CreditID=618, Status='P'}</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2150,10 +2547,14 @@
         <v>691</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=19, DegreePlanSelected=7082, Term=4, CreditID=691, Status='P'}</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2167,10 +2568,14 @@
         <v>20</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=20, DegreePlanSelected=7082, Term=4, CreditID=20, Status='P'}</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2184,10 +2589,14 @@
         <v>692</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=21, DegreePlanSelected=7082, Term=5, CreditID=692, Status='P'}</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2201,10 +2610,14 @@
         <v>555</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=22, DegreePlanSelected=7082, Term=5, CreditID=555, Status='P'}</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2218,10 +2631,14 @@
         <v>542</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=23, DegreePlanSelected=8973, Term=1, CreditID=542, Status='A'}</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2235,10 +2652,14 @@
         <v>563</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=24, DegreePlanSelected=8973, Term=1, CreditID=563, Status='A'}</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2252,10 +2673,14 @@
         <v>560</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=25, DegreePlanSelected=8973, Term=1, CreditID=560, Status='A'}</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2269,10 +2694,14 @@
         <v>664</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=26, DegreePlanSelected=8973, Term=2, CreditID=664, Status='P'}</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2286,10 +2715,14 @@
         <v>6</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=27, DegreePlanSelected=8973, Term=2, CreditID=6, Status='P'}</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2303,10 +2736,14 @@
         <v>10</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=28, DegreePlanSelected=8973, Term=2, CreditID=10, Status='P'}</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2320,10 +2757,14 @@
         <v>20</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=29, DegreePlanSelected=8973, Term=3, CreditID=20, Status='P'}</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2337,10 +2778,14 @@
         <v>555</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=30, DegreePlanSelected=8973, Term=3, CreditID=555, Status='P'}</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2354,10 +2799,14 @@
         <v>691</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=31, DegreePlanSelected=8973, Term=3, CreditID=691, Status='P'}</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2371,10 +2820,14 @@
         <v>618</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=32, DegreePlanSelected=8973, Term=4, CreditID=618, Status='P'}</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2388,7 +2841,11 @@
         <v>692</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="F34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>new Slot {SlotID=33, DegreePlanSelected=8973, Term=4, CreditID=692, Status='P'}</v>
       </c>
     </row>
   </sheetData>
@@ -2398,10 +2855,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2410,26 +2867,30 @@
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="65.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2440,13 +2901,17 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F2" t="str">
+        <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A2 &amp; ", " &amp;$B$1 &amp;"=" &amp;B2 &amp; ", "&amp;$C$1 &amp;"=" &amp;C2 &amp; ", "&amp;$D$1 &amp;"='" &amp;D2 &amp; "', "&amp;$E$1 &amp;"='" &amp;E2 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTermID=1, StudentId=533568, Term=1, TermAbbr='F18', TermName='Fall 2018'}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2457,13 +2922,17 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F14" si="0">"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A3 &amp; ", " &amp;$B$1 &amp;"=" &amp;B3 &amp; ", "&amp;$C$1 &amp;"=" &amp;C3 &amp; ", "&amp;$D$1 &amp;"='" &amp;D3 &amp; "', "&amp;$E$1 &amp;"='" &amp;E3 &amp;"'}"</f>
+        <v>new StudentTerm {StudentTermID=2, StudentId=533568, Term=2, TermAbbr='SP19', TermName='Spring 2019'}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2474,13 +2943,17 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm {StudentTermID=3, StudentId=533568, Term=3, TermAbbr='SU19', TermName='Summer 2019'}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2491,13 +2964,17 @@
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm {StudentTermID=4, StudentId=533568, Term=4, TermAbbr='F19', TermName='Fall 2019'}</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2508,13 +2985,17 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm {StudentTermID=5, StudentId=533708, Term=1, TermAbbr='F18', TermName='Fall 2018'}</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2525,13 +3006,17 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm {StudentTermID=6, StudentId=533708, Term=2, TermAbbr='SP19', TermName='Spring 2019'}</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2542,13 +3027,17 @@
         <v>3</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm {StudentTermID=7, StudentId=533708, Term=3, TermAbbr='SU19', TermName='Summer 2019'}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2559,13 +3048,17 @@
         <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm {StudentTermID=8, StudentId=533708, Term=4, TermAbbr='F19', TermName='Fall 2019'}</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2576,13 +3069,17 @@
         <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm {StudentTermID=9, StudentId=533708, Term=5, TermAbbr='SP20', TermName='Spring 2020'}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2593,13 +3090,17 @@
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm {StudentTermID=10, StudentId=533897, Term=1, TermAbbr='SP20', TermName='Spring 2020'}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2610,13 +3111,17 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm {StudentTermID=11, StudentId=533897, Term=2, TermAbbr='FA20', TermName='Fall 2020'}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2627,13 +3132,17 @@
         <v>3</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm {StudentTermID=12, StudentId=533897, Term=3, TermAbbr='SP21', TermName='Spring 2021'}</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2644,10 +3153,14 @@
         <v>4</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>new StudentTerm {StudentTermID=13, StudentId=533897, Term=4, TermAbbr='SU21', TermName='Summer 2021'}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ordered seeding according to foreign key req. Updated Excel data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="88">
   <si>
     <t>DegreeID</t>
   </si>
@@ -180,9 +180,6 @@
   </si>
   <si>
     <t>StudentTermID</t>
-  </si>
-  <si>
-    <t>StudentId</t>
   </si>
   <si>
     <t>TermAbbr</t>
@@ -631,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -648,16 +645,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -776,7 +773,7 @@
         <v>34</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1114,7 +1111,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1123,7 +1120,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1871,22 +1868,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1900,7 +1897,7 @@
         <v>40</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="2">
         <v>5681</v>
@@ -1918,10 +1915,10 @@
         <v>533568</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3" s="2">
         <v>5682</v>
@@ -1942,7 +1939,7 @@
         <v>40</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="2">
         <v>7081</v>
@@ -1960,10 +1957,10 @@
         <v>533708</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" s="2">
         <v>7082</v>
@@ -1984,7 +1981,7 @@
         <v>40</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="2">
         <v>8971</v>
@@ -2002,10 +1999,10 @@
         <v>533897</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="E7" s="2">
         <v>8973</v>
@@ -2053,10 +2050,10 @@
         <v>42</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2064,10 +2061,10 @@
         <v>533568</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="D2" s="3">
         <v>919569870</v>
@@ -2082,10 +2079,10 @@
         <v>533708</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="D3" s="3">
         <v>919571315</v>
@@ -2100,10 +2097,10 @@
         <v>533897</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="D4" s="3">
         <v>919571233</v>
@@ -2123,7 +2120,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2140,7 +2137,7 @@
         <v>48</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>43</v>
@@ -2152,7 +2149,7 @@
         <v>44</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2858,7 +2855,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2875,19 +2872,19 @@
         <v>49</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2901,14 +2898,14 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="F2" t="str">
         <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A2 &amp; ", " &amp;$B$1 &amp;"=" &amp;B2 &amp; ", "&amp;$C$1 &amp;"=" &amp;C2 &amp; ", "&amp;$D$1 &amp;"='" &amp;D2 &amp; "', "&amp;$E$1 &amp;"='" &amp;E2 &amp;"'}"</f>
-        <v>new StudentTerm {StudentTermID=1, StudentId=533568, Term=1, TermAbbr='F18', TermName='Fall 2018'}</v>
+        <v>new StudentTerm {StudentTermID=1, StudentID=533568, Term=1, TermAbbr='F18', TermName='Fall 2018'}</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2922,14 +2919,14 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F14" si="0">"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A3 &amp; ", " &amp;$B$1 &amp;"=" &amp;B3 &amp; ", "&amp;$C$1 &amp;"=" &amp;C3 &amp; ", "&amp;$D$1 &amp;"='" &amp;D3 &amp; "', "&amp;$E$1 &amp;"='" &amp;E3 &amp;"'}"</f>
-        <v>new StudentTerm {StudentTermID=2, StudentId=533568, Term=2, TermAbbr='SP19', TermName='Spring 2019'}</v>
+        <v>new StudentTerm {StudentTermID=2, StudentID=533568, Term=2, TermAbbr='SP19', TermName='Spring 2019'}</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2943,14 +2940,14 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=3, StudentId=533568, Term=3, TermAbbr='SU19', TermName='Summer 2019'}</v>
+        <v>new StudentTerm {StudentTermID=3, StudentID=533568, Term=3, TermAbbr='SU19', TermName='Summer 2019'}</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2964,14 +2961,14 @@
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=4, StudentId=533568, Term=4, TermAbbr='F19', TermName='Fall 2019'}</v>
+        <v>new StudentTerm {StudentTermID=4, StudentID=533568, Term=4, TermAbbr='F19', TermName='Fall 2019'}</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2985,14 +2982,14 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=5, StudentId=533708, Term=1, TermAbbr='F18', TermName='Fall 2018'}</v>
+        <v>new StudentTerm {StudentTermID=5, StudentID=533708, Term=1, TermAbbr='F18', TermName='Fall 2018'}</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3006,14 +3003,14 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=6, StudentId=533708, Term=2, TermAbbr='SP19', TermName='Spring 2019'}</v>
+        <v>new StudentTerm {StudentTermID=6, StudentID=533708, Term=2, TermAbbr='SP19', TermName='Spring 2019'}</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3027,14 +3024,14 @@
         <v>3</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=7, StudentId=533708, Term=3, TermAbbr='SU19', TermName='Summer 2019'}</v>
+        <v>new StudentTerm {StudentTermID=7, StudentID=533708, Term=3, TermAbbr='SU19', TermName='Summer 2019'}</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3048,14 +3045,14 @@
         <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=8, StudentId=533708, Term=4, TermAbbr='F19', TermName='Fall 2019'}</v>
+        <v>new StudentTerm {StudentTermID=8, StudentID=533708, Term=4, TermAbbr='F19', TermName='Fall 2019'}</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3069,14 +3066,14 @@
         <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=9, StudentId=533708, Term=5, TermAbbr='SP20', TermName='Spring 2020'}</v>
+        <v>new StudentTerm {StudentTermID=9, StudentID=533708, Term=5, TermAbbr='SP20', TermName='Spring 2020'}</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3090,14 +3087,14 @@
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=10, StudentId=533897, Term=1, TermAbbr='SP20', TermName='Spring 2020'}</v>
+        <v>new StudentTerm {StudentTermID=10, StudentID=533897, Term=1, TermAbbr='SP20', TermName='Spring 2020'}</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3111,14 +3108,14 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=11, StudentId=533897, Term=2, TermAbbr='FA20', TermName='Fall 2020'}</v>
+        <v>new StudentTerm {StudentTermID=11, StudentID=533897, Term=2, TermAbbr='FA20', TermName='Fall 2020'}</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3132,14 +3129,14 @@
         <v>3</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=12, StudentId=533897, Term=3, TermAbbr='SP21', TermName='Spring 2021'}</v>
+        <v>new StudentTerm {StudentTermID=12, StudentID=533897, Term=3, TermAbbr='SP21', TermName='Spring 2021'}</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3153,14 +3150,14 @@
         <v>4</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=13, StudentId=533897, Term=4, TermAbbr='SU21', TermName='Summer 2021'}</v>
+        <v>new StudentTerm {StudentTermID=13, StudentID=533897, Term=4, TermAbbr='SU21', TermName='Summer 2021'}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added DatabaseGeneratedOption to NONE Data seeded
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,8 +671,8 @@
         <v>4</v>
       </c>
       <c r="E2" t="str">
-        <f>"new Degree {" &amp;$A$1 &amp;" = " &amp;A2 &amp; ", " &amp;$B$1 &amp; "='" &amp;B2  &amp; "', " &amp;$C$1 &amp; "='" &amp;C2 &amp;"'}"</f>
-        <v>new Degree {DegreeID = 1, DegreeAbbr='ACS+2', DegreeName='MS ACS+2'}</v>
+        <f>"new Degree {" &amp;$A$1 &amp;" = " &amp;A2 &amp; ", " &amp;$B$1 &amp; "='" &amp;B2  &amp; "', " &amp;$C$1 &amp; "='" &amp;C2 &amp;"', "&amp;$D$1 &amp; "=" &amp;D2&amp;"}"</f>
+        <v>new Degree {DegreeID = 1, DegreeAbbr='ACS+2', DegreeName='MS ACS+2', NumberOfTerms=4}</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -689,8 +689,8 @@
         <v>4</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E5" si="0">"new Degree {" &amp;$A$1 &amp;" = " &amp;A3 &amp; ", " &amp;$B$1 &amp; "='" &amp;B3  &amp; "', " &amp;$C$1 &amp; "='" &amp;C3 &amp;"'"</f>
-        <v>new Degree {DegreeID = 2, DegreeAbbr='ACS+DB', DegreeName='MS ACS+DB'</v>
+        <f t="shared" ref="E3:E5" si="0">"new Degree {" &amp;$A$1 &amp;" = " &amp;A3 &amp; ", " &amp;$B$1 &amp; "='" &amp;B3  &amp; "', " &amp;$C$1 &amp; "='" &amp;C3 &amp;"', "&amp;$D$1 &amp; "=" &amp;D3&amp;"}"</f>
+        <v>new Degree {DegreeID = 2, DegreeAbbr='ACS+DB', DegreeName='MS ACS+DB', NumberOfTerms=4}</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -708,7 +708,7 @@
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>new Degree {DegreeID = 3, DegreeAbbr='ACS+NF', DegreeName='MS ACS+NF'</v>
+        <v>new Degree {DegreeID = 3, DegreeAbbr='ACS+NF', DegreeName='MS ACS+NF', NumberOfTerms=4}</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -726,7 +726,7 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>new Degree {DegreeID = 4, DegreeAbbr='ACS', DegreeName='MS ACS'</v>
+        <v>new Degree {DegreeID = 4, DegreeAbbr='ACS', DegreeName='MS ACS', NumberOfTerms=4}</v>
       </c>
     </row>
   </sheetData>
@@ -2854,7 +2854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
column names updated in excel
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="88">
   <si>
-    <t>DegreeID</t>
-  </si>
-  <si>
     <t>ACS+2</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>NumberOfTerms</t>
   </si>
   <si>
-    <t>CreditID</t>
-  </si>
-  <si>
     <t>CreditAbbr</t>
   </si>
   <si>
@@ -149,9 +143,6 @@
     <t>Elective 2</t>
   </si>
   <si>
-    <t>StudentID</t>
-  </si>
-  <si>
     <t>Super Fast</t>
   </si>
   <si>
@@ -176,12 +167,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>SlotID</t>
-  </si>
-  <si>
-    <t>StudentTermID</t>
-  </si>
-  <si>
     <t>TermAbbr</t>
   </si>
   <si>
@@ -269,9 +254,6 @@
     <t>Summer 2021</t>
   </si>
   <si>
-    <t>DegreePlanID</t>
-  </si>
-  <si>
     <t>DegreePlanAbbr</t>
   </si>
   <si>
@@ -281,9 +263,6 @@
     <t>DegreePlanSelected</t>
   </si>
   <si>
-    <t>DegreeCreditID</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -294,6 +273,27 @@
   </si>
   <si>
     <t>N919</t>
+  </si>
+  <si>
+    <t>DegreeId</t>
+  </si>
+  <si>
+    <t>CreditId</t>
+  </si>
+  <si>
+    <t>DegreeCreditId</t>
+  </si>
+  <si>
+    <t>DegreePlanId</t>
+  </si>
+  <si>
+    <t>StudentId</t>
+  </si>
+  <si>
+    <t>SlotId</t>
+  </si>
+  <si>
+    <t>StudentTermId</t>
   </si>
 </sst>
 </file>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E5"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,19 +642,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -662,17 +662,17 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="3">
         <v>4</v>
       </c>
       <c r="E2" t="str">
         <f>"new Degree {" &amp;$A$1 &amp;" = " &amp;A2 &amp; ", " &amp;$B$1 &amp; "='" &amp;B2  &amp; "', " &amp;$C$1 &amp; "='" &amp;C2 &amp;"', "&amp;$D$1 &amp; "=" &amp;D2&amp;"}"</f>
-        <v>new Degree {DegreeID = 1, DegreeAbbr='ACS+2', DegreeName='MS ACS+2', NumberOfTerms=4}</v>
+        <v>new Degree {DegreeId = 1, DegreeAbbr='ACS+2', DegreeName='MS ACS+2', NumberOfTerms=4}</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -680,17 +680,17 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3">
         <v>4</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E5" si="0">"new Degree {" &amp;$A$1 &amp;" = " &amp;A3 &amp; ", " &amp;$B$1 &amp; "='" &amp;B3  &amp; "', " &amp;$C$1 &amp; "='" &amp;C3 &amp;"', "&amp;$D$1 &amp; "=" &amp;D3&amp;"}"</f>
-        <v>new Degree {DegreeID = 2, DegreeAbbr='ACS+DB', DegreeName='MS ACS+DB', NumberOfTerms=4}</v>
+        <v>new Degree {DegreeId = 2, DegreeAbbr='ACS+DB', DegreeName='MS ACS+DB', NumberOfTerms=4}</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -698,17 +698,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="3">
         <v>4</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>new Degree {DegreeID = 3, DegreeAbbr='ACS+NF', DegreeName='MS ACS+NF', NumberOfTerms=4}</v>
+        <v>new Degree {DegreeId = 3, DegreeAbbr='ACS+NF', DegreeName='MS ACS+NF', NumberOfTerms=4}</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -716,17 +716,17 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3">
         <v>4</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>new Degree {DegreeID = 4, DegreeAbbr='ACS', DegreeName='MS ACS', NumberOfTerms=4}</v>
+        <v>new Degree {DegreeId = 4, DegreeAbbr='ACS', DegreeName='MS ACS', NumberOfTerms=4}</v>
       </c>
     </row>
   </sheetData>
@@ -740,7 +740,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,25 +755,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="D1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -781,10 +781,10 @@
         <v>460</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -797,7 +797,7 @@
       </c>
       <c r="G2" s="3" t="str">
         <f>"new Credit {" &amp;$A$1 &amp;"=" &amp;A2 &amp; ", " &amp;$B$1 &amp;"='" &amp;B2 &amp; "', " &amp;$C$1 &amp;"='" &amp;C2 &amp; "', "&amp;$D$1 &amp;"=" &amp;D2 &amp; ", "&amp;$E$1 &amp;"=" &amp;E2 &amp; ", " &amp;$F$1 &amp;"=" &amp;F2 &amp;"}"</f>
-        <v>new Credit {CreditID=460, CreditAbbr='DB', CreditName='Databases', IsSummer=0, IsSpring=1, IsFall=1}</v>
+        <v>new Credit {CreditId=460, CreditAbbr='DB', CreditName='Databases', IsSummer=0, IsSpring=1, IsFall=1}</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -805,10 +805,10 @@
         <v>356</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
@@ -821,7 +821,7 @@
       </c>
       <c r="G3" s="3" t="str">
         <f t="shared" ref="G3:G14" si="0">"new Credit {" &amp;$A$1 &amp;"=" &amp;A3 &amp; ", " &amp;$B$1 &amp;"='" &amp;B3 &amp; "', " &amp;$C$1 &amp;"='" &amp;C3 &amp; "', "&amp;$D$1 &amp;"=" &amp;D3 &amp; ", "&amp;$E$1 &amp;"=" &amp;E3 &amp; ", " &amp;$F$1 &amp;"=" &amp;F3 &amp;"}"</f>
-        <v>new Credit {CreditID=356, CreditAbbr='NF', CreditName='Network Fundamentals', IsSummer=0, IsSpring=1, IsFall=1}</v>
+        <v>new Credit {CreditId=356, CreditAbbr='NF', CreditName='Network Fundamentals', IsSummer=0, IsSpring=1, IsFall=1}</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -832,7 +832,7 @@
         <v>542</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -845,7 +845,7 @@
       </c>
       <c r="G4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Credit {CreditID=542, CreditAbbr='542', CreditName='OOPS with Java', IsSummer=0, IsSpring=1, IsFall=1}</v>
+        <v>new Credit {CreditId=542, CreditAbbr='542', CreditName='OOPS with Java', IsSummer=0, IsSpring=1, IsFall=1}</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -856,7 +856,7 @@
         <v>563</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -869,7 +869,7 @@
       </c>
       <c r="G5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Credit {CreditID=563, CreditAbbr='563', CreditName='Web Apps', IsSummer=0, IsSpring=1, IsFall=1}</v>
+        <v>new Credit {CreditId=563, CreditAbbr='563', CreditName='Web Apps', IsSummer=0, IsSpring=1, IsFall=1}</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -880,7 +880,7 @@
         <v>560</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>1</v>
@@ -893,7 +893,7 @@
       </c>
       <c r="G6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Credit {CreditID=560, CreditAbbr='560', CreditName='Advanced Databases', IsSummer=1, IsSpring=1, IsFall=1}</v>
+        <v>new Credit {CreditId=560, CreditAbbr='560', CreditName='Advanced Databases', IsSummer=1, IsSpring=1, IsFall=1}</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -901,10 +901,10 @@
         <v>664</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -917,7 +917,7 @@
       </c>
       <c r="G7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Credit {CreditID=664, CreditAbbr='664-UX', CreditName='User Experience', IsSummer=0, IsSpring=1, IsFall=1}</v>
+        <v>new Credit {CreditId=664, CreditAbbr='664-UX', CreditName='User Experience', IsSummer=0, IsSpring=1, IsFall=1}</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -925,10 +925,10 @@
         <v>618</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
@@ -941,7 +941,7 @@
       </c>
       <c r="G8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Credit {CreditID=618, CreditAbbr='618-PM', CreditName='Project Management', IsSummer=1, IsSpring=0, IsFall=0}</v>
+        <v>new Credit {CreditId=618, CreditAbbr='618-PM', CreditName='Project Management', IsSummer=1, IsSpring=0, IsFall=0}</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -949,10 +949,10 @@
         <v>555</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -965,7 +965,7 @@
       </c>
       <c r="G9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Credit {CreditID=555, CreditAbbr='555-NS', CreditName='Network Security', IsSummer=0, IsSpring=1, IsFall=1}</v>
+        <v>new Credit {CreditId=555, CreditAbbr='555-NS', CreditName='Network Security', IsSummer=0, IsSpring=1, IsFall=1}</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -973,10 +973,10 @@
         <v>691</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -989,7 +989,7 @@
       </c>
       <c r="G10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Credit {CreditID=691, CreditAbbr='691-GDP1', CreditName='GDP1', IsSummer=0, IsSpring=1, IsFall=1}</v>
+        <v>new Credit {CreditId=691, CreditAbbr='691-GDP1', CreditName='GDP1', IsSummer=0, IsSpring=1, IsFall=1}</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -997,10 +997,10 @@
         <v>692</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="G11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Credit {CreditID=692, CreditAbbr='692-GDP2', CreditName='GDP2', IsSummer=0, IsSpring=1, IsFall=1}</v>
+        <v>new Credit {CreditId=692, CreditAbbr='692-GDP2', CreditName='GDP2', IsSummer=0, IsSpring=1, IsFall=1}</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1021,10 +1021,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" s="3">
         <v>0</v>
@@ -1037,7 +1037,7 @@
       </c>
       <c r="G12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Credit {CreditID=6, CreditAbbr='Mobile', CreditName='643 or 644 Mobile', IsSummer=0, IsSpring=1, IsFall=1}</v>
+        <v>new Credit {CreditId=6, CreditAbbr='Mobile', CreditName='643 or 644 Mobile', IsSummer=0, IsSpring=1, IsFall=1}</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1045,10 +1045,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="D13" s="3">
         <v>0</v>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="G13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Credit {CreditID=10, CreditAbbr='E1', CreditName='Elective 1', IsSummer=0, IsSpring=1, IsFall=1}</v>
+        <v>new Credit {CreditId=10, CreditAbbr='E1', CreditName='Elective 1', IsSummer=0, IsSpring=1, IsFall=1}</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1069,10 +1069,10 @@
         <v>20</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="D14" s="3">
         <v>0</v>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="G14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Credit {CreditID=20, CreditAbbr='E2', CreditName='Elective 2', IsSummer=0, IsSpring=1, IsFall=1}</v>
+        <v>new Credit {CreditId=20, CreditAbbr='E2', CreditName='Elective 2', IsSummer=0, IsSpring=1, IsFall=1}</v>
       </c>
     </row>
   </sheetData>
@@ -1098,7 +1098,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,13 +1114,13 @@
         <v>83</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1135,7 +1135,7 @@
       </c>
       <c r="D2" s="3" t="str">
         <f>"new DegreeCredit {" &amp;$A$1 &amp;"=" &amp;A2 &amp; ", " &amp;$B$1 &amp;"=" &amp;B2 &amp; ", " &amp;$C$1 &amp;"=" &amp;C2 &amp;"}"</f>
-        <v>new DegreeCredit {DegreeCreditID=1, DegreeID=1, CreditID=460}</v>
+        <v>new DegreeCredit {DegreeCreditId=1, DegreeId=1, CreditId=460}</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="D3" s="3" t="str">
         <f t="shared" ref="D3:D49" si="0">"new DegreeCredit {" &amp;$A$1 &amp;"=" &amp;A3 &amp; ", " &amp;$B$1 &amp;"=" &amp;B3 &amp; ", " &amp;$C$1 &amp;"=" &amp;C3 &amp;"}"</f>
-        <v>new DegreeCredit {DegreeCreditID=2, DegreeID=1, CreditID=356}</v>
+        <v>new DegreeCredit {DegreeCreditId=2, DegreeId=1, CreditId=356}</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=3, DegreeID=1, CreditID=542}</v>
+        <v>new DegreeCredit {DegreeCreditId=3, DegreeId=1, CreditId=542}</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1180,7 +1180,7 @@
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=4, DegreeID=1, CreditID=563}</v>
+        <v>new DegreeCredit {DegreeCreditId=4, DegreeId=1, CreditId=563}</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=5, DegreeID=1, CreditID=560}</v>
+        <v>new DegreeCredit {DegreeCreditId=5, DegreeId=1, CreditId=560}</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1210,7 +1210,7 @@
       </c>
       <c r="D7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=6, DegreeID=1, CreditID=664}</v>
+        <v>new DegreeCredit {DegreeCreditId=6, DegreeId=1, CreditId=664}</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1225,7 +1225,7 @@
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=7, DegreeID=1, CreditID=618}</v>
+        <v>new DegreeCredit {DegreeCreditId=7, DegreeId=1, CreditId=618}</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=8, DegreeID=1, CreditID=555}</v>
+        <v>new DegreeCredit {DegreeCreditId=8, DegreeId=1, CreditId=555}</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1255,7 +1255,7 @@
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=9, DegreeID=1, CreditID=691}</v>
+        <v>new DegreeCredit {DegreeCreditId=9, DegreeId=1, CreditId=691}</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=10, DegreeID=1, CreditID=692}</v>
+        <v>new DegreeCredit {DegreeCreditId=10, DegreeId=1, CreditId=692}</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=11, DegreeID=1, CreditID=6}</v>
+        <v>new DegreeCredit {DegreeCreditId=11, DegreeId=1, CreditId=6}</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="D13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=12, DegreeID=1, CreditID=10}</v>
+        <v>new DegreeCredit {DegreeCreditId=12, DegreeId=1, CreditId=10}</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1315,7 +1315,7 @@
       </c>
       <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=13, DegreeID=1, CreditID=20}</v>
+        <v>new DegreeCredit {DegreeCreditId=13, DegreeId=1, CreditId=20}</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="D15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=14, DegreeID=2, CreditID=460}</v>
+        <v>new DegreeCredit {DegreeCreditId=14, DegreeId=2, CreditId=460}</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1345,7 +1345,7 @@
       </c>
       <c r="D16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=15, DegreeID=2, CreditID=542}</v>
+        <v>new DegreeCredit {DegreeCreditId=15, DegreeId=2, CreditId=542}</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1360,7 +1360,7 @@
       </c>
       <c r="D17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=16, DegreeID=2, CreditID=563}</v>
+        <v>new DegreeCredit {DegreeCreditId=16, DegreeId=2, CreditId=563}</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=17, DegreeID=2, CreditID=560}</v>
+        <v>new DegreeCredit {DegreeCreditId=17, DegreeId=2, CreditId=560}</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1390,7 +1390,7 @@
       </c>
       <c r="D19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=18, DegreeID=2, CreditID=664}</v>
+        <v>new DegreeCredit {DegreeCreditId=18, DegreeId=2, CreditId=664}</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1405,7 +1405,7 @@
       </c>
       <c r="D20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=19, DegreeID=2, CreditID=618}</v>
+        <v>new DegreeCredit {DegreeCreditId=19, DegreeId=2, CreditId=618}</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1420,7 +1420,7 @@
       </c>
       <c r="D21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=20, DegreeID=2, CreditID=555}</v>
+        <v>new DegreeCredit {DegreeCreditId=20, DegreeId=2, CreditId=555}</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="D22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=21, DegreeID=2, CreditID=691}</v>
+        <v>new DegreeCredit {DegreeCreditId=21, DegreeId=2, CreditId=691}</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1450,7 +1450,7 @@
       </c>
       <c r="D23" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=22, DegreeID=2, CreditID=692}</v>
+        <v>new DegreeCredit {DegreeCreditId=22, DegreeId=2, CreditId=692}</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="D24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=23, DegreeID=2, CreditID=6}</v>
+        <v>new DegreeCredit {DegreeCreditId=23, DegreeId=2, CreditId=6}</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1480,7 +1480,7 @@
       </c>
       <c r="D25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=24, DegreeID=2, CreditID=10}</v>
+        <v>new DegreeCredit {DegreeCreditId=24, DegreeId=2, CreditId=10}</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="D26" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=25, DegreeID=2, CreditID=20}</v>
+        <v>new DegreeCredit {DegreeCreditId=25, DegreeId=2, CreditId=20}</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1510,7 +1510,7 @@
       </c>
       <c r="D27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=26, DegreeID=3, CreditID=356}</v>
+        <v>new DegreeCredit {DegreeCreditId=26, DegreeId=3, CreditId=356}</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1525,7 +1525,7 @@
       </c>
       <c r="D28" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=27, DegreeID=3, CreditID=542}</v>
+        <v>new DegreeCredit {DegreeCreditId=27, DegreeId=3, CreditId=542}</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1540,7 +1540,7 @@
       </c>
       <c r="D29" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=28, DegreeID=3, CreditID=563}</v>
+        <v>new DegreeCredit {DegreeCreditId=28, DegreeId=3, CreditId=563}</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1555,7 +1555,7 @@
       </c>
       <c r="D30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=29, DegreeID=3, CreditID=560}</v>
+        <v>new DegreeCredit {DegreeCreditId=29, DegreeId=3, CreditId=560}</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1570,7 +1570,7 @@
       </c>
       <c r="D31" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=30, DegreeID=3, CreditID=664}</v>
+        <v>new DegreeCredit {DegreeCreditId=30, DegreeId=3, CreditId=664}</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1585,7 +1585,7 @@
       </c>
       <c r="D32" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=31, DegreeID=3, CreditID=618}</v>
+        <v>new DegreeCredit {DegreeCreditId=31, DegreeId=3, CreditId=618}</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1600,7 +1600,7 @@
       </c>
       <c r="D33" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=32, DegreeID=3, CreditID=555}</v>
+        <v>new DegreeCredit {DegreeCreditId=32, DegreeId=3, CreditId=555}</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1615,7 +1615,7 @@
       </c>
       <c r="D34" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=33, DegreeID=3, CreditID=691}</v>
+        <v>new DegreeCredit {DegreeCreditId=33, DegreeId=3, CreditId=691}</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1630,7 +1630,7 @@
       </c>
       <c r="D35" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=34, DegreeID=3, CreditID=692}</v>
+        <v>new DegreeCredit {DegreeCreditId=34, DegreeId=3, CreditId=692}</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1645,7 +1645,7 @@
       </c>
       <c r="D36" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=35, DegreeID=3, CreditID=6}</v>
+        <v>new DegreeCredit {DegreeCreditId=35, DegreeId=3, CreditId=6}</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1660,7 +1660,7 @@
       </c>
       <c r="D37" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=36, DegreeID=3, CreditID=10}</v>
+        <v>new DegreeCredit {DegreeCreditId=36, DegreeId=3, CreditId=10}</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1675,7 +1675,7 @@
       </c>
       <c r="D38" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=37, DegreeID=3, CreditID=20}</v>
+        <v>new DegreeCredit {DegreeCreditId=37, DegreeId=3, CreditId=20}</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1690,7 +1690,7 @@
       </c>
       <c r="D39" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=38, DegreeID=4, CreditID=542}</v>
+        <v>new DegreeCredit {DegreeCreditId=38, DegreeId=4, CreditId=542}</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1705,7 +1705,7 @@
       </c>
       <c r="D40" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=39, DegreeID=4, CreditID=563}</v>
+        <v>new DegreeCredit {DegreeCreditId=39, DegreeId=4, CreditId=563}</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1720,7 +1720,7 @@
       </c>
       <c r="D41" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=40, DegreeID=4, CreditID=560}</v>
+        <v>new DegreeCredit {DegreeCreditId=40, DegreeId=4, CreditId=560}</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1735,7 +1735,7 @@
       </c>
       <c r="D42" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=41, DegreeID=4, CreditID=664}</v>
+        <v>new DegreeCredit {DegreeCreditId=41, DegreeId=4, CreditId=664}</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="D43" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=42, DegreeID=4, CreditID=618}</v>
+        <v>new DegreeCredit {DegreeCreditId=42, DegreeId=4, CreditId=618}</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
       </c>
       <c r="D44" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=43, DegreeID=4, CreditID=555}</v>
+        <v>new DegreeCredit {DegreeCreditId=43, DegreeId=4, CreditId=555}</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1780,7 +1780,7 @@
       </c>
       <c r="D45" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=44, DegreeID=4, CreditID=691}</v>
+        <v>new DegreeCredit {DegreeCreditId=44, DegreeId=4, CreditId=691}</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1795,7 +1795,7 @@
       </c>
       <c r="D46" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=45, DegreeID=4, CreditID=692}</v>
+        <v>new DegreeCredit {DegreeCreditId=45, DegreeId=4, CreditId=692}</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1810,7 +1810,7 @@
       </c>
       <c r="D47" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=46, DegreeID=4, CreditID=6}</v>
+        <v>new DegreeCredit {DegreeCreditId=46, DegreeId=4, CreditId=6}</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1825,7 +1825,7 @@
       </c>
       <c r="D48" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=47, DegreeID=4, CreditID=10}</v>
+        <v>new DegreeCredit {DegreeCreditId=47, DegreeId=4, CreditId=10}</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1840,7 +1840,7 @@
       </c>
       <c r="D49" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreeCredit {DegreeCreditID=48, DegreeID=4, CreditID=20}</v>
+        <v>new DegreeCredit {DegreeCreditId=48, DegreeId=4, CreditId=20}</v>
       </c>
     </row>
   </sheetData>
@@ -1853,7 +1853,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1868,22 +1868,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1894,17 +1894,17 @@
         <v>533568</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E2" s="2">
         <v>5681</v>
       </c>
       <c r="F2" t="str">
         <f>"new DegreePlan {" &amp;$A$1 &amp;"=" &amp;A2 &amp; ", " &amp;$B$1 &amp;"=" &amp;B2 &amp; ", " &amp;$C$1 &amp;"='" &amp;C2 &amp; "', "&amp;$D$1 &amp;"='" &amp;D2 &amp; "', "&amp;$E$1 &amp;"=" &amp;E2 &amp; "}"</f>
-        <v>new DegreePlan {DegreePlanID=1, StudentID=533568, DegreePlanAbbr='Super Fast', DegreePlanName='Cheetah', DegreePlanSelected=5681}</v>
+        <v>new DegreePlan {DegreePlanId=1, StudentId=533568, DegreePlanAbbr='Super Fast', DegreePlanName='Cheetah', DegreePlanSelected=5681}</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1915,17 +1915,17 @@
         <v>533568</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E3" s="2">
         <v>5682</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F7" si="0">"new DegreePlan {" &amp;$A$1 &amp;"=" &amp;A3 &amp; ", " &amp;$B$1 &amp;"=" &amp;B3 &amp; ", " &amp;$C$1 &amp;"='" &amp;C3 &amp; "', "&amp;$D$1 &amp;"='" &amp;D3 &amp; "', "&amp;$E$1 &amp;"=" &amp;E3 &amp; "}"</f>
-        <v>new DegreePlan {DegreePlanID=2, StudentID=533568, DegreePlanAbbr='Slow and Easy', DegreePlanName='Tortoise', DegreePlanSelected=5682}</v>
+        <v>new DegreePlan {DegreePlanId=2, StudentId=533568, DegreePlanAbbr='Slow and Easy', DegreePlanName='Tortoise', DegreePlanSelected=5682}</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1936,17 +1936,17 @@
         <v>533708</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E4" s="2">
         <v>7081</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlan {DegreePlanID=3, StudentID=533708, DegreePlanAbbr='Super Fast', DegreePlanName='Cheetah', DegreePlanSelected=7081}</v>
+        <v>new DegreePlan {DegreePlanId=3, StudentId=533708, DegreePlanAbbr='Super Fast', DegreePlanName='Cheetah', DegreePlanSelected=7081}</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1957,17 +1957,17 @@
         <v>533708</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E5" s="2">
         <v>7082</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlan {DegreePlanID=4, StudentID=533708, DegreePlanAbbr='Slow and Easy', DegreePlanName='Tortoise', DegreePlanSelected=7082}</v>
+        <v>new DegreePlan {DegreePlanId=4, StudentId=533708, DegreePlanAbbr='Slow and Easy', DegreePlanName='Tortoise', DegreePlanSelected=7082}</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1978,17 +1978,17 @@
         <v>533897</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E6" s="2">
         <v>8971</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlan {DegreePlanID=5, StudentID=533897, DegreePlanAbbr='Super Fast', DegreePlanName='Cheetah', DegreePlanSelected=8971}</v>
+        <v>new DegreePlan {DegreePlanId=5, StudentId=533897, DegreePlanAbbr='Super Fast', DegreePlanName='Cheetah', DegreePlanSelected=8971}</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1999,17 +1999,17 @@
         <v>533897</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E7" s="2">
         <v>8973</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>new DegreePlan {DegreePlanID=6, StudentID=533897, DegreePlanAbbr='Summer Off', DegreePlanName='Rabbit', DegreePlanSelected=8973}</v>
+        <v>new DegreePlan {DegreePlanId=6, StudentId=533897, DegreePlanAbbr='Summer Off', DegreePlanName='Rabbit', DegreePlanSelected=8973}</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2025,9 +2025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2041,19 +2039,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2061,17 +2059,17 @@
         <v>533568</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D2" s="3">
         <v>919569870</v>
       </c>
       <c r="E2" s="3" t="str">
         <f>"new Student {" &amp;$A$1 &amp;"=" &amp;A2 &amp; ", " &amp;$B$1 &amp;"='" &amp;B2 &amp; "', "&amp;$C$1 &amp;"='" &amp;C2 &amp; "', "&amp;$D$1 &amp;"=" &amp;D2 &amp;"}"</f>
-        <v>new Student {StudentID=533568, Family='Bodepudi', Given='Mallikarjuna', N919=919569870}</v>
+        <v>new Student {StudentId=533568, Family='Bodepudi', Given='Mallikarjuna', N919=919569870}</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2079,17 +2077,17 @@
         <v>533708</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D3" s="3">
         <v>919571315</v>
       </c>
       <c r="E3" s="3" t="str">
         <f t="shared" ref="E3:E4" si="0">"new Student {" &amp;$A$1 &amp;"=" &amp;A3 &amp; ", " &amp;$B$1 &amp;"='" &amp;B3 &amp; "', "&amp;$C$1 &amp;"='" &amp;C3 &amp; "', "&amp;$D$1 &amp;"=" &amp;D3 &amp;"}"</f>
-        <v>new Student {StudentID=533708, Family='Kancharla', Given='Sai Krishna Teja', N919=919571315}</v>
+        <v>new Student {StudentId=533708, Family='Kancharla', Given='Sai Krishna Teja', N919=919571315}</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2097,17 +2095,17 @@
         <v>533897</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D4" s="3">
         <v>919571233</v>
       </c>
       <c r="E4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Student {StudentID=533897, Family='Atluri', Given='Mouni Krishna', N919=919571233}</v>
+        <v>new Student {StudentId=533897, Family='Atluri', Given='Mouni Krishna', N919=919571233}</v>
       </c>
     </row>
   </sheetData>
@@ -2120,7 +2118,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2134,22 +2132,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2166,11 +2164,11 @@
         <v>542</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F2" s="3" t="str">
         <f>"new Slot {" &amp;$A$1 &amp;"=" &amp;A2 &amp; ", " &amp;$B$1 &amp;"=" &amp;B2 &amp; ", "&amp;$C$1 &amp;"=" &amp;C2 &amp; ", "&amp;$D$1 &amp;"=" &amp;D2 &amp; ", "&amp;$E$1 &amp;"='" &amp;E2 &amp;"'}"</f>
-        <v>new Slot {SlotID=1, DegreePlanSelected=5681, Term=1, CreditID=542, Status='C'}</v>
+        <v>new Slot {SlotId=1, DegreePlanSelected=5681, Term=1, CreditId=542, Status='C'}</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2187,11 +2185,11 @@
         <v>563</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F3" s="3" t="str">
         <f t="shared" ref="F3:F34" si="0">"new Slot {" &amp;$A$1 &amp;"=" &amp;A3 &amp; ", " &amp;$B$1 &amp;"=" &amp;B3 &amp; ", "&amp;$C$1 &amp;"=" &amp;C3 &amp; ", "&amp;$D$1 &amp;"=" &amp;D3 &amp; ", "&amp;$E$1 &amp;"='" &amp;E3 &amp;"'}"</f>
-        <v>new Slot {SlotID=2, DegreePlanSelected=5681, Term=1, CreditID=563, Status='C'}</v>
+        <v>new Slot {SlotId=2, DegreePlanSelected=5681, Term=1, CreditId=563, Status='C'}</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2208,11 +2206,11 @@
         <v>560</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=3, DegreePlanSelected=5681, Term=1, CreditID=560, Status='C'}</v>
+        <v>new Slot {SlotId=3, DegreePlanSelected=5681, Term=1, CreditId=560, Status='C'}</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2229,11 +2227,11 @@
         <v>664</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=4, DegreePlanSelected=5681, Term=2, CreditID=664, Status='A'}</v>
+        <v>new Slot {SlotId=4, DegreePlanSelected=5681, Term=2, CreditId=664, Status='A'}</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2250,11 +2248,11 @@
         <v>6</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=5, DegreePlanSelected=5681, Term=2, CreditID=6, Status='A'}</v>
+        <v>new Slot {SlotId=5, DegreePlanSelected=5681, Term=2, CreditId=6, Status='A'}</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2271,11 +2269,11 @@
         <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=6, DegreePlanSelected=5681, Term=2, CreditID=10, Status='A'}</v>
+        <v>new Slot {SlotId=6, DegreePlanSelected=5681, Term=2, CreditId=10, Status='A'}</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2292,11 +2290,11 @@
         <v>618</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=7, DegreePlanSelected=5681, Term=3, CreditID=618, Status='P'}</v>
+        <v>new Slot {SlotId=7, DegreePlanSelected=5681, Term=3, CreditId=618, Status='P'}</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2313,11 +2311,11 @@
         <v>691</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=8, DegreePlanSelected=5681, Term=3, CreditID=691, Status='P'}</v>
+        <v>new Slot {SlotId=8, DegreePlanSelected=5681, Term=3, CreditId=691, Status='P'}</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2334,11 +2332,11 @@
         <v>692</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=9, DegreePlanSelected=5681, Term=4, CreditID=692, Status='P'}</v>
+        <v>new Slot {SlotId=9, DegreePlanSelected=5681, Term=4, CreditId=692, Status='P'}</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2355,11 +2353,11 @@
         <v>20</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=10, DegreePlanSelected=5681, Term=4, CreditID=20, Status='P'}</v>
+        <v>new Slot {SlotId=10, DegreePlanSelected=5681, Term=4, CreditId=20, Status='P'}</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2376,11 +2374,11 @@
         <v>555</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=11, DegreePlanSelected=5681, Term=4, CreditID=555, Status='P'}</v>
+        <v>new Slot {SlotId=11, DegreePlanSelected=5681, Term=4, CreditId=555, Status='P'}</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2397,11 +2395,11 @@
         <v>542</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=12, DegreePlanSelected=7082, Term=1, CreditID=542, Status='C'}</v>
+        <v>new Slot {SlotId=12, DegreePlanSelected=7082, Term=1, CreditId=542, Status='C'}</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2418,11 +2416,11 @@
         <v>563</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=13, DegreePlanSelected=7082, Term=1, CreditID=563, Status='C'}</v>
+        <v>new Slot {SlotId=13, DegreePlanSelected=7082, Term=1, CreditId=563, Status='C'}</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2439,11 +2437,11 @@
         <v>560</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=14, DegreePlanSelected=7082, Term=1, CreditID=560, Status='C'}</v>
+        <v>new Slot {SlotId=14, DegreePlanSelected=7082, Term=1, CreditId=560, Status='C'}</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2460,11 +2458,11 @@
         <v>664</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=15, DegreePlanSelected=7082, Term=2, CreditID=664, Status='A'}</v>
+        <v>new Slot {SlotId=15, DegreePlanSelected=7082, Term=2, CreditId=664, Status='A'}</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2481,11 +2479,11 @@
         <v>6</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=16, DegreePlanSelected=7082, Term=2, CreditID=6, Status='A'}</v>
+        <v>new Slot {SlotId=16, DegreePlanSelected=7082, Term=2, CreditId=6, Status='A'}</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2502,11 +2500,11 @@
         <v>10</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=17, DegreePlanSelected=7082, Term=2, CreditID=10, Status='A'}</v>
+        <v>new Slot {SlotId=17, DegreePlanSelected=7082, Term=2, CreditId=10, Status='A'}</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2523,11 +2521,11 @@
         <v>618</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=18, DegreePlanSelected=7082, Term=3, CreditID=618, Status='P'}</v>
+        <v>new Slot {SlotId=18, DegreePlanSelected=7082, Term=3, CreditId=618, Status='P'}</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2544,11 +2542,11 @@
         <v>691</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=19, DegreePlanSelected=7082, Term=4, CreditID=691, Status='P'}</v>
+        <v>new Slot {SlotId=19, DegreePlanSelected=7082, Term=4, CreditId=691, Status='P'}</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2565,11 +2563,11 @@
         <v>20</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=20, DegreePlanSelected=7082, Term=4, CreditID=20, Status='P'}</v>
+        <v>new Slot {SlotId=20, DegreePlanSelected=7082, Term=4, CreditId=20, Status='P'}</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2586,11 +2584,11 @@
         <v>692</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=21, DegreePlanSelected=7082, Term=5, CreditID=692, Status='P'}</v>
+        <v>new Slot {SlotId=21, DegreePlanSelected=7082, Term=5, CreditId=692, Status='P'}</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2607,11 +2605,11 @@
         <v>555</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F23" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=22, DegreePlanSelected=7082, Term=5, CreditID=555, Status='P'}</v>
+        <v>new Slot {SlotId=22, DegreePlanSelected=7082, Term=5, CreditId=555, Status='P'}</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2628,11 +2626,11 @@
         <v>542</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=23, DegreePlanSelected=8973, Term=1, CreditID=542, Status='A'}</v>
+        <v>new Slot {SlotId=23, DegreePlanSelected=8973, Term=1, CreditId=542, Status='A'}</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2649,11 +2647,11 @@
         <v>563</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=24, DegreePlanSelected=8973, Term=1, CreditID=563, Status='A'}</v>
+        <v>new Slot {SlotId=24, DegreePlanSelected=8973, Term=1, CreditId=563, Status='A'}</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2670,11 +2668,11 @@
         <v>560</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F26" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=25, DegreePlanSelected=8973, Term=1, CreditID=560, Status='A'}</v>
+        <v>new Slot {SlotId=25, DegreePlanSelected=8973, Term=1, CreditId=560, Status='A'}</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2691,11 +2689,11 @@
         <v>664</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=26, DegreePlanSelected=8973, Term=2, CreditID=664, Status='P'}</v>
+        <v>new Slot {SlotId=26, DegreePlanSelected=8973, Term=2, CreditId=664, Status='P'}</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2712,11 +2710,11 @@
         <v>6</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F28" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=27, DegreePlanSelected=8973, Term=2, CreditID=6, Status='P'}</v>
+        <v>new Slot {SlotId=27, DegreePlanSelected=8973, Term=2, CreditId=6, Status='P'}</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2733,11 +2731,11 @@
         <v>10</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F29" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=28, DegreePlanSelected=8973, Term=2, CreditID=10, Status='P'}</v>
+        <v>new Slot {SlotId=28, DegreePlanSelected=8973, Term=2, CreditId=10, Status='P'}</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2754,11 +2752,11 @@
         <v>20</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=29, DegreePlanSelected=8973, Term=3, CreditID=20, Status='P'}</v>
+        <v>new Slot {SlotId=29, DegreePlanSelected=8973, Term=3, CreditId=20, Status='P'}</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2775,11 +2773,11 @@
         <v>555</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F31" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=30, DegreePlanSelected=8973, Term=3, CreditID=555, Status='P'}</v>
+        <v>new Slot {SlotId=30, DegreePlanSelected=8973, Term=3, CreditId=555, Status='P'}</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2796,11 +2794,11 @@
         <v>691</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F32" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=31, DegreePlanSelected=8973, Term=3, CreditID=691, Status='P'}</v>
+        <v>new Slot {SlotId=31, DegreePlanSelected=8973, Term=3, CreditId=691, Status='P'}</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2817,11 +2815,11 @@
         <v>618</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F33" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=32, DegreePlanSelected=8973, Term=4, CreditID=618, Status='P'}</v>
+        <v>new Slot {SlotId=32, DegreePlanSelected=8973, Term=4, CreditId=618, Status='P'}</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2838,11 +2836,11 @@
         <v>692</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F34" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>new Slot {SlotID=33, DegreePlanSelected=8973, Term=4, CreditID=692, Status='P'}</v>
+        <v>new Slot {SlotId=33, DegreePlanSelected=8973, Term=4, CreditId=692, Status='P'}</v>
       </c>
     </row>
   </sheetData>
@@ -2854,8 +2852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2869,22 +2867,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2898,14 +2896,14 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F2" t="str">
         <f>"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A2 &amp; ", " &amp;$B$1 &amp;"=" &amp;B2 &amp; ", "&amp;$C$1 &amp;"=" &amp;C2 &amp; ", "&amp;$D$1 &amp;"='" &amp;D2 &amp; "', "&amp;$E$1 &amp;"='" &amp;E2 &amp;"'}"</f>
-        <v>new StudentTerm {StudentTermID=1, StudentID=533568, Term=1, TermAbbr='F18', TermName='Fall 2018'}</v>
+        <v>new StudentTerm {StudentTermId=1, StudentId=533568, Term=1, TermAbbr='F18', TermName='Fall 2018'}</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2919,14 +2917,14 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F14" si="0">"new StudentTerm {" &amp;$A$1 &amp;"=" &amp;A3 &amp; ", " &amp;$B$1 &amp;"=" &amp;B3 &amp; ", "&amp;$C$1 &amp;"=" &amp;C3 &amp; ", "&amp;$D$1 &amp;"='" &amp;D3 &amp; "', "&amp;$E$1 &amp;"='" &amp;E3 &amp;"'}"</f>
-        <v>new StudentTerm {StudentTermID=2, StudentID=533568, Term=2, TermAbbr='SP19', TermName='Spring 2019'}</v>
+        <v>new StudentTerm {StudentTermId=2, StudentId=533568, Term=2, TermAbbr='SP19', TermName='Spring 2019'}</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2940,14 +2938,14 @@
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=3, StudentID=533568, Term=3, TermAbbr='SU19', TermName='Summer 2019'}</v>
+        <v>new StudentTerm {StudentTermId=3, StudentId=533568, Term=3, TermAbbr='SU19', TermName='Summer 2019'}</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2961,14 +2959,14 @@
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=4, StudentID=533568, Term=4, TermAbbr='F19', TermName='Fall 2019'}</v>
+        <v>new StudentTerm {StudentTermId=4, StudentId=533568, Term=4, TermAbbr='F19', TermName='Fall 2019'}</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2982,14 +2980,14 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=5, StudentID=533708, Term=1, TermAbbr='F18', TermName='Fall 2018'}</v>
+        <v>new StudentTerm {StudentTermId=5, StudentId=533708, Term=1, TermAbbr='F18', TermName='Fall 2018'}</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3003,14 +3001,14 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=6, StudentID=533708, Term=2, TermAbbr='SP19', TermName='Spring 2019'}</v>
+        <v>new StudentTerm {StudentTermId=6, StudentId=533708, Term=2, TermAbbr='SP19', TermName='Spring 2019'}</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3024,14 +3022,14 @@
         <v>3</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=7, StudentID=533708, Term=3, TermAbbr='SU19', TermName='Summer 2019'}</v>
+        <v>new StudentTerm {StudentTermId=7, StudentId=533708, Term=3, TermAbbr='SU19', TermName='Summer 2019'}</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3045,14 +3043,14 @@
         <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=8, StudentID=533708, Term=4, TermAbbr='F19', TermName='Fall 2019'}</v>
+        <v>new StudentTerm {StudentTermId=8, StudentId=533708, Term=4, TermAbbr='F19', TermName='Fall 2019'}</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3066,14 +3064,14 @@
         <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=9, StudentID=533708, Term=5, TermAbbr='SP20', TermName='Spring 2020'}</v>
+        <v>new StudentTerm {StudentTermId=9, StudentId=533708, Term=5, TermAbbr='SP20', TermName='Spring 2020'}</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3087,14 +3085,14 @@
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=10, StudentID=533897, Term=1, TermAbbr='SP20', TermName='Spring 2020'}</v>
+        <v>new StudentTerm {StudentTermId=10, StudentId=533897, Term=1, TermAbbr='SP20', TermName='Spring 2020'}</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3108,14 +3106,14 @@
         <v>2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=11, StudentID=533897, Term=2, TermAbbr='FA20', TermName='Fall 2020'}</v>
+        <v>new StudentTerm {StudentTermId=11, StudentId=533897, Term=2, TermAbbr='FA20', TermName='Fall 2020'}</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3129,14 +3127,14 @@
         <v>3</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=12, StudentID=533897, Term=3, TermAbbr='SP21', TermName='Spring 2021'}</v>
+        <v>new StudentTerm {StudentTermId=12, StudentId=533897, Term=3, TermAbbr='SP21', TermName='Spring 2021'}</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3150,14 +3148,14 @@
         <v>4</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>new StudentTerm {StudentTermID=13, StudentID=533897, Term=4, TermAbbr='SU21', TermName='Summer 2021'}</v>
+        <v>new StudentTerm {StudentTermId=13, StudentId=533897, Term=4, TermAbbr='SU21', TermName='Summer 2021'}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>